<commit_message>
changes to the judge algorithm - Assign all hearing days first based on UA (#6859)
</commit_message>
<xml_diff>
--- a/spec/support/singleNonAvailJudgeSpreadsheet.xlsx
+++ b/spec/support/singleNonAvailJudgeSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarramirez/caseflow/spec/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vacogivenc/Developer/gov.va/caseflow-certification/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5A305E-760B-D841-9005-A2C28352FA45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{81D5F496-1374-6B47-9314-D5CD66DB8F4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33200" yWindow="3020" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17640" yWindow="3020" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Judge Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -66,22 +66,26 @@
       <sz val="14"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="13"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1615,7 +1619,7 @@
   <dimension ref="A1:IV8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1755,7 +1759,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="29">
-        <v>43312</v>
+        <v>43311</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="4"/>

</xml_diff>